<commit_message>
Fix Excel si no recibe clave
</commit_message>
<xml_diff>
--- a/public/assets/files/PlantillaProductos.xlsx
+++ b/public/assets/files/PlantillaProductos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissa/Dropbox/PHORMO/phormo-equipo/Clientes/eTax/app - plantillas excel/versión agosto/con categoría/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAC962B-7FCE-4899-9B20-37026F68B07C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508DE7BF-6887-DC4F-A2C5-97681F581485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4515" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="-680" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,779 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Usuario de Microsoft Office</author>
+    <author>eTax</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{2CB27E77-6DE1-774C-BA7A-D438F643109B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Código de producto:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El código de producto es un código definido por usted que se utiliza para ordenar sus productos en eTax.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Defina un código nuevo para productos nuevos.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="1" shapeId="0" xr:uid="{FFDA3C34-876C-624A-9C6B-3EFA1CB4C2AA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Códigos de IVA de eTax:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Consulte nuestro </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Manual de códigos de eTax </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>para conocer cuál es el código correspondiente a la línea de factura.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="6"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>Encuentre nuestro manual en nuestro centro de soporte (https://etaxcr.com/soporte/) o directamente dentro de su sesión de eTax.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="6"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{3893B822-9C74-9044-AE60-3902A441083A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Categoría de declaración:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Digite el número que corresponde a la categoría de declaración requerida.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">*Importante: Verifique que la categoría elegida corresponda con el Código de IVA de eTax seleccionado.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">1 Bienes generales al 1% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">2 Bienes de capital al 1% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">3 Servicios al 1% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">4 Uso o consumo personal de mercancias y servicios al 1% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">5 Transferencias sin contraprestación a terceros 1% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">6 Medicamentos, materias primas, insumos, maquinaria, equipo y reactivos para su producción 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">7 Primas de seguros personales 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">8 Bienes y servicios que hagan las instituciones estatales de educación superior y otras autorizadas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">9 Otros servicios de educación privada no acreditados por el MEP y/o CONESUP 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">10 Boletos o pasajes aéreos nacionales 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">11 Boletos o pasajes aéreos internacionales 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">12 Servicios de salud privados 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">13 Servicios de ingeniería, arquitectura, topografía, y construcción de obra civil 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">14 Servicios de recolección, clasificación y almacenamiento de bienes reciclables y reutilizables, insc… 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">15 Bienes generales al 13% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">16 Bienes de capital al 13% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">17 Servicios al 13% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">18 Uso o consumo personal de mercancias y servicios al 13% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">19 Transferencias sin contraprestación a terceros 13% 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">20 Incrementos en la base imponible por recaudación a nivel de mayorista 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">21 Servicios adquiridos desde el exterior 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">22 Exportaciones de bienes 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">23 Exportaciones de servicios 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">24 Venta local de bienes exentos 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">25 Venta local de servicios exentos 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">26 Créditos para descuentos de facturas y arrendamientos financieros 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">27 Arrendamientos destinados a viviendas y accesorios, así como los lugares de culto religioso 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">28 Arrendamientos utilizados por micro y pequeñas empresas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">29 Suministro de energía eléctrica residencial no mayor a 280 KW/H 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">30 Venta o entrega de agua residencial no mayor a 30 M3 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">31 Autoconsumo de bienes y servicios sin aplicación de créditos total o parcial 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">32 Venta de sillas de ruedas y similares, equipo ortopédico, prótesis y equipo 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">33 Venta de bienes y servicios a instituciones públicas y privadas exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">34 Aranceles por matrícula y créditos de cursos en universidades públicas y privadas exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">35 Servicios de transporte terrestre de pasajeros y cabotaje de personas con concesión 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">36 Venta, arrendamiento y leasing de autobuses y embarcaciones 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">37 Comisiones por el servicio de subasta ganadera y transacción de animales 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">38 Venta, comercialización y matanza de animales vivos 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">39 Ventas sin impuesto a clientes autorizados por la Dirección General de Hacienda 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">40 Ventas sin impuesto a clientes autorizados por la Dirección General de Tributación 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">41 Ventas sin impuesto a clientes exonerados por ley especial 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">42 Ventas de bienes y servicios relacionados a la canasta básica tributaria exentos el 1er año de la le… 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">43 Servicios de ingeniería, arquitectura, topografía y construcción de obra civil con planos visados an… 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">44 Servicios turísticos inscritos ante el Instituto Costarricense de Turismo 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">45 Servicios de recolección, clasificación y almacenamiento de bienes reciclables y reutilizables, insc… 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">46 Bienes y servicios a la Caja Costarricense de Seguro Social 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">47 Bienes y servicios a las corporaciones municipales 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">48 Otras ventas no sujetas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">49 Compras locales de bienes utilizados en operaciones sujetas y no exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">50 Compras locales de servicios utilizados en operaciones sujetas y no exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">51 Compras locales de bienes de capital utilizados en operaciones sujetas y no exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">52 Importaciones de bienes utilizados en operaciones sujetas y no exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">53 Importaciones de servicios utilizados en operaciones sujetas y no exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">54 Importaciones de bienes de capital utilizados en operaciones sujetas y no exentas 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">55 Compras locales de bienes y servicios exentos 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">56 Importaciones de bienes y servicios exentos 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">57 Compras locales de bienes y servicios no relacionados directamente con la actividad 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">58 Importaciones de bienes y servicios no relacionados directamente con la actividad 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">59 Compras de bienes con IVA no acreditable por gastos no deducibles </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Codigo</t>
   </si>
@@ -50,13 +821,63 @@
   </si>
   <si>
     <t>CodigoEtax</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bienvenido al sistema de importación de productos vía excel de eTax. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+Complete los datos de sus proveedores en las celdas correspondientes (a partir de la fila 4, inclusive). Cada producto se detalla en su propia fila.
+Pase su cursor por las celdas de la segunda fila marcadas con un triángulo en la esquina superior derecha para ver más detalles sobre la información que debe digitar.
+No modifique los textos de la tercera fila. Estos son necesarios para la correcta lectura del documento.</t>
+    </r>
+  </si>
+  <si>
+    <t>Indique la unidad de medida utilizada para cuantificar el producto.</t>
+  </si>
+  <si>
+    <t>Indique el precio del producto.</t>
+  </si>
+  <si>
+    <t>Indique el nombre del producto.</t>
+  </si>
+  <si>
+    <t>Indique el código de producto utilizado en eTax.</t>
+  </si>
+  <si>
+    <t>Indique la descripción del producto</t>
+  </si>
+  <si>
+    <t>Indique el código de IVA de eTax típicamente correspondiente al producto.</t>
+  </si>
+  <si>
+    <t>B103</t>
+  </si>
+  <si>
+    <t>Indique el código correspondiente a la categoría de declaración ante Ministerio de Hacienda.</t>
+  </si>
+  <si>
+    <t>CategoriaDeclaracion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -68,6 +889,80 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -96,9 +991,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,7 +1028,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,63 +1323,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="5" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="79" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="49" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D4">
         <v>2300</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>103</v>
+      <c r="F4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>